<commit_message>
new migration and BD manuals BD units
</commit_message>
<xml_diff>
--- a/public/data/bd_avia_v3_a.xlsx
+++ b/public/data/bd_avia_v3_a.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\avia.loc\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\avia.loc\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEC9A139-B3A2-4D03-9991-0EEA1FA4CCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="1725" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="1725" windowWidth="24240" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="128">
   <si>
     <t>workorder</t>
   </si>
@@ -397,9 +396,6 @@
     <t>component_tdr</t>
   </si>
   <si>
-    <t>training_name</t>
-  </si>
-  <si>
     <t>training_hours</t>
   </si>
   <si>
@@ -407,12 +403,18 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>unit_name_training</t>
+  </si>
+  <si>
+    <t>unit_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1110,58 +1112,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1182,9 +1148,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,25 +1169,64 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Form # 003" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal_Form # 003" xfId="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1501,11 +1503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,8 +1519,8 @@
     <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="28" style="9" customWidth="1"/>
     <col min="7" max="7" width="1.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="0.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="29" style="1" bestFit="1" customWidth="1"/>
@@ -1535,27 +1537,27 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="E2" s="74" t="s">
+      <c r="C2" s="104"/>
+      <c r="E2" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="H2" s="69" t="s">
+      <c r="F2" s="104"/>
+      <c r="H2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="70"/>
+      <c r="I2" s="93"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="85"/>
-      <c r="N2" s="69" t="s">
+      <c r="L2" s="89"/>
+      <c r="N2" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="70"/>
+      <c r="O2" s="93"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
@@ -1635,10 +1637,10 @@
       <c r="F5" s="13"/>
       <c r="G5" s="2"/>
       <c r="H5" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" s="33" t="s">
         <v>125</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>126</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="14" t="s">
@@ -1678,10 +1680,10 @@
       <c r="L6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="78" t="s">
+      <c r="N6" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="79"/>
+      <c r="O6" s="95"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
@@ -1727,10 +1729,10 @@
       <c r="F8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="79"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="5"/>
       <c r="K8" s="35"/>
       <c r="L8" s="36"/>
@@ -1784,10 +1786,10 @@
         <v>66</v>
       </c>
       <c r="J10" s="5"/>
-      <c r="N10" s="80" t="s">
+      <c r="N10" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="81"/>
+      <c r="O10" s="91"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
@@ -1880,16 +1882,16 @@
         <v>53</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="I14" s="33" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="3"/>
-      <c r="N14" s="80" t="s">
+      <c r="N14" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="81"/>
+      <c r="O14" s="91"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
@@ -1901,7 +1903,7 @@
         <v>53</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I15" s="33" t="s">
         <v>18</v>
@@ -1920,11 +1922,11 @@
       <c r="F16" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>35</v>
+      <c r="H16" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>18</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>5</v>
@@ -1934,10 +1936,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="72"/>
+      <c r="C17" s="101"/>
       <c r="E17" s="31" t="s">
         <v>6</v>
       </c>
@@ -1968,10 +1970,10 @@
       <c r="I18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="80" t="s">
+      <c r="N18" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="81"/>
+      <c r="O18" s="91"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
@@ -2074,10 +2076,10 @@
       <c r="D25" s="27"/>
       <c r="E25" s="2"/>
       <c r="F25" s="7"/>
-      <c r="N25" s="80" t="s">
+      <c r="N25" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="81"/>
+      <c r="O25" s="91"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="28"/>
@@ -2105,20 +2107,20 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="73"/>
+      <c r="C28" s="102"/>
       <c r="D28" s="48"/>
-      <c r="E28" s="82" t="s">
+      <c r="E28" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="86"/>
+      <c r="F28" s="105"/>
       <c r="G28" s="48"/>
-      <c r="H28" s="82" t="s">
+      <c r="H28" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="I28" s="83"/>
+      <c r="I28" s="99"/>
       <c r="N28" s="18"/>
       <c r="O28" s="24"/>
     </row>
@@ -2143,10 +2145,10 @@
       <c r="I29" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="80" t="s">
+      <c r="N29" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="81"/>
+      <c r="O29" s="91"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="63" t="s">
@@ -2184,10 +2186,10 @@
         <v>27</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="87" t="s">
+      <c r="E31" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="76"/>
       <c r="G31" s="2"/>
       <c r="H31" s="16" t="s">
         <v>11</v>
@@ -2210,8 +2212,8 @@
         <v>27</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="90"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="2"/>
       <c r="H32" s="16" t="s">
         <v>119</v>
@@ -2230,8 +2232,8 @@
         <v>53</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="90"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="78"/>
       <c r="G33" s="2"/>
       <c r="H33" s="16" t="s">
         <v>120</v>
@@ -2239,17 +2241,17 @@
       <c r="I33" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="80" t="s">
+      <c r="N33" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="81"/>
+      <c r="O33" s="91"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="67"/>
       <c r="C34" s="29"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="90"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="78"/>
       <c r="G34" s="2"/>
       <c r="H34" s="64"/>
       <c r="I34" s="46"/>
@@ -2264,8 +2266,8 @@
       <c r="B35" s="67"/>
       <c r="C35" s="29"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="90"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="78"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="50"/>
@@ -2280,24 +2282,24 @@
       <c r="B36" s="49"/>
       <c r="C36" s="30"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="90"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="78"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="105" t="s">
+      <c r="H36" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="93"/>
-      <c r="N36" s="76" t="s">
+      <c r="I36" s="74"/>
+      <c r="N36" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="77"/>
+      <c r="O36" s="97"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="49"/>
       <c r="C37" s="7"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="90"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="78"/>
       <c r="G37" s="2"/>
       <c r="H37" s="10" t="s">
         <v>20</v>
@@ -2313,13 +2315,13 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="94"/>
+      <c r="C38" s="81"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="90"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="78"/>
       <c r="G38" s="2"/>
       <c r="H38" s="38" t="s">
         <v>5</v>
@@ -2342,8 +2344,8 @@
         <v>22</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="90"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="2"/>
       <c r="H39" s="38" t="s">
         <v>25</v>
@@ -2362,22 +2364,22 @@
         <v>18</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="90"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="78"/>
       <c r="G40" s="2"/>
       <c r="H40" s="18"/>
       <c r="I40" s="50"/>
-      <c r="N40" s="76" t="s">
+      <c r="N40" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="O40" s="77"/>
+      <c r="O40" s="97"/>
     </row>
     <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="49"/>
       <c r="C41" s="7"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="90"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="78"/>
       <c r="G41" s="2"/>
       <c r="H41" s="41" t="s">
         <v>85</v>
@@ -2393,13 +2395,13 @@
       </c>
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="95" t="s">
+      <c r="B42" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="96"/>
+      <c r="C42" s="83"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="90"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="78"/>
       <c r="G42" s="2"/>
       <c r="H42" s="41" t="s">
         <v>87</v>
@@ -2415,13 +2417,13 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="97" t="s">
+      <c r="B43" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="98"/>
+      <c r="C43" s="85"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="90"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="78"/>
       <c r="G43" s="2"/>
       <c r="H43" s="41" t="s">
         <v>89</v>
@@ -2431,13 +2433,13 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="97" t="s">
+      <c r="B44" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="98"/>
+      <c r="C44" s="85"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="90"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="78"/>
       <c r="G44" s="2"/>
       <c r="H44" s="41" t="s">
         <v>91</v>
@@ -2447,13 +2449,13 @@
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="99" t="s">
+      <c r="B45" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="100"/>
+      <c r="C45" s="87"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="90"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="78"/>
       <c r="G45" s="2"/>
       <c r="H45" s="41" t="s">
         <v>93</v>
@@ -2466,8 +2468,8 @@
       <c r="B46" s="56"/>
       <c r="C46" s="57"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="90"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="78"/>
       <c r="G46" s="2"/>
       <c r="H46" s="41" t="s">
         <v>95</v>
@@ -2477,13 +2479,13 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="93" t="s">
+      <c r="B47" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="94"/>
+      <c r="C47" s="81"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="90"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="78"/>
       <c r="G47" s="2"/>
       <c r="H47" s="41" t="s">
         <v>97</v>
@@ -2500,8 +2502,8 @@
         <v>22</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="90"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="78"/>
       <c r="G48" s="2"/>
       <c r="H48" s="41" t="s">
         <v>99</v>
@@ -2518,8 +2520,8 @@
         <v>27</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="92"/>
+      <c r="E49" s="79"/>
+      <c r="F49" s="80"/>
       <c r="G49" s="2"/>
       <c r="H49" s="41" t="s">
         <v>101</v>
@@ -2543,10 +2545,10 @@
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="101" t="s">
+      <c r="B51" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="102"/>
+      <c r="C51" s="70"/>
       <c r="D51" s="2"/>
       <c r="E51" s="68"/>
       <c r="F51" s="68"/>
@@ -2559,10 +2561,10 @@
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="101" t="s">
+      <c r="B52" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="102"/>
+      <c r="C52" s="70"/>
       <c r="D52" s="2"/>
       <c r="E52" s="68"/>
       <c r="F52" s="68"/>
@@ -2575,10 +2577,10 @@
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="102"/>
+      <c r="C53" s="70"/>
       <c r="D53" s="2"/>
       <c r="E53" s="68"/>
       <c r="F53" s="68"/>
@@ -2591,10 +2593,10 @@
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="101" t="s">
+      <c r="B54" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="102"/>
+      <c r="C54" s="70"/>
       <c r="D54" s="2"/>
       <c r="E54" s="68"/>
       <c r="F54" s="68"/>
@@ -2607,10 +2609,10 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="101" t="s">
+      <c r="B55" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="102"/>
+      <c r="C55" s="70"/>
       <c r="D55" s="2"/>
       <c r="E55" s="68"/>
       <c r="F55" s="68"/>
@@ -2619,10 +2621,10 @@
       <c r="I55" s="50"/>
     </row>
     <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="103" t="s">
+      <c r="B56" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="104"/>
+      <c r="C56" s="72"/>
       <c r="D56" s="2"/>
       <c r="E56" s="68"/>
       <c r="F56" s="68"/>
@@ -2672,6 +2674,25 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N14:O14"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="H36:I36"/>
@@ -2686,25 +2707,6 @@
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
@@ -2712,7 +2714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add: -UnitTDR -UnitTDR-migration -Component-migration add manual_id
</commit_message>
<xml_diff>
--- a/public/data/bd_avia_v3_a.xlsx
+++ b/public/data/bd_avia_v3_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\avia\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC818AC1-48D9-4FC1-87F2-5E3FDF575F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFBE5A4-98F7-46C5-8245-B48A2D103B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="166">
   <si>
     <t>workorder</t>
   </si>
@@ -450,6 +450,117 @@
 LOCKWIRE DAMAGE (MISSING) FROME ,
  CORRODED at/on,
  SPRING (S)</t>
+  </si>
+  <si>
+    <t>DAMAGED IN AREA OF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THREADS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORRODED  at/on  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORN BEYOND LIMITS IN THE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHIMMED INCORRECTLY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ELECTRO-HYDROLIC SERVO VALVE INOPERATIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OUT OF ADJUSTMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONTAMINATED WITH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CYLINDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SEAL (S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BEARING (S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PISTON CHROME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONNECTOR DAMAGED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNIT OPERATING NOISY DUE TO </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WIRE (s)  DAMAGED IN AREA OF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BEARING JOURNAL WORN BEYOND LIMITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BEARING LINER WORN BEYOND LIMITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AXLE ASSY (BEARING JOURNALS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AXLE ASSY (PISTON BORE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UPPER TORQUE LINK ASSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOWER TORQUE LINK ASSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MAIN FTTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRUNNION PINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PISTON CROSS PIN HOLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INSTALLATION BORE OF THE BUSHING </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNIT COULD NOT EXTEND AND LOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> THE PAINT FINISH - </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L.V.D.T - INOPERATIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LIVE TIME IS EXPIRED </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UPON ARRIVAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOCKWIRE DAMAGE (MISSING) FROME </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CORRODED at/on</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SPRING (S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEAKING FROM</t>
+  </si>
+  <si>
+    <t>? SOLENOID INOPERATIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PISTON</t>
   </si>
 </sst>
 </file>
@@ -914,7 +1025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1078,6 +1189,60 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1117,68 +1282,18 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1467,7 +1582,7 @@
   <dimension ref="B1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:I60"/>
+      <selection activeCell="E31" sqref="E31:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,27 +1609,27 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="E2" s="83" t="s">
+      <c r="C2" s="61"/>
+      <c r="E2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="H2" s="72" t="s">
+      <c r="F2" s="61"/>
+      <c r="H2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="73"/>
+      <c r="I2" s="56"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="69"/>
-      <c r="N2" s="72" t="s">
+      <c r="L2" s="72"/>
+      <c r="N2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="73"/>
+      <c r="O2" s="56"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1633,10 +1748,10 @@
       <c r="L6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="74" t="s">
+      <c r="N6" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="75"/>
+      <c r="O6" s="67"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1680,10 +1795,10 @@
       <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="74" t="s">
+      <c r="H8" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="67"/>
       <c r="J8" s="2"/>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -1737,10 +1852,10 @@
         <v>66</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="N10" s="70" t="s">
+      <c r="N10" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="71"/>
+      <c r="O10" s="69"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -1839,10 +1954,10 @@
         <v>18</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="N14" s="70" t="s">
+      <c r="N14" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="71"/>
+      <c r="O14" s="69"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
@@ -1885,10 +2000,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="81"/>
+      <c r="C17" s="58"/>
       <c r="E17" s="24" t="s">
         <v>6</v>
       </c>
@@ -1919,10 +2034,10 @@
       <c r="I18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="70" t="s">
+      <c r="N18" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="71"/>
+      <c r="O18" s="69"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
@@ -2022,10 +2137,10 @@
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
       <c r="D25" s="21"/>
-      <c r="N25" s="70" t="s">
+      <c r="N25" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="71"/>
+      <c r="O25" s="69"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
@@ -2048,20 +2163,20 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="82" t="s">
+      <c r="B28" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="78" t="s">
+      <c r="E28" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="85"/>
+      <c r="F28" s="63"/>
       <c r="G28" s="35"/>
-      <c r="H28" s="78" t="s">
+      <c r="H28" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="I28" s="79"/>
+      <c r="I28" s="70"/>
       <c r="N28" s="12"/>
       <c r="O28" s="18"/>
     </row>
@@ -2084,10 +2199,10 @@
       <c r="I29" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="70" t="s">
+      <c r="N29" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="71"/>
+      <c r="O29" s="69"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="50" t="s">
@@ -2172,10 +2287,10 @@
       <c r="I33" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="N33" s="70" t="s">
+      <c r="N33" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="71"/>
+      <c r="O33" s="69"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="54"/>
@@ -2208,14 +2323,14 @@
       <c r="B36" s="36"/>
       <c r="E36" s="87"/>
       <c r="F36" s="87"/>
-      <c r="H36" s="59" t="s">
+      <c r="H36" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="I36" s="60"/>
-      <c r="N36" s="76" t="s">
+      <c r="I36" s="78"/>
+      <c r="N36" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="77"/>
+      <c r="O36" s="65"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="36"/>
@@ -2235,10 +2350,10 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="61"/>
+      <c r="C38" s="79"/>
       <c r="E38" s="87"/>
       <c r="F38" s="87"/>
       <c r="H38" s="27" t="s">
@@ -2283,10 +2398,10 @@
       <c r="F40" s="87"/>
       <c r="H40" s="12"/>
       <c r="I40" s="37"/>
-      <c r="N40" s="76" t="s">
+      <c r="N40" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="O40" s="77"/>
+      <c r="O40" s="65"/>
     </row>
     <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="36"/>
@@ -2306,10 +2421,10 @@
       </c>
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="63"/>
+      <c r="C42" s="81"/>
       <c r="E42" s="87"/>
       <c r="F42" s="87"/>
       <c r="H42" s="30" t="s">
@@ -2326,10 +2441,10 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="65"/>
+      <c r="C43" s="83"/>
       <c r="E43" s="87"/>
       <c r="F43" s="87"/>
       <c r="H43" s="30" t="s">
@@ -2340,10 +2455,10 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="64" t="s">
+      <c r="B44" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="65"/>
+      <c r="C44" s="83"/>
       <c r="E44" s="87"/>
       <c r="F44" s="87"/>
       <c r="H44" s="30" t="s">
@@ -2354,10 +2469,10 @@
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="66" t="s">
+      <c r="B45" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="67"/>
+      <c r="C45" s="85"/>
       <c r="E45" s="87"/>
       <c r="F45" s="87"/>
       <c r="H45" s="30" t="s">
@@ -2380,10 +2495,10 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="60" t="s">
+      <c r="B47" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="61"/>
+      <c r="C47" s="79"/>
       <c r="E47" s="87"/>
       <c r="F47" s="87"/>
       <c r="H47" s="30" t="s">
@@ -2438,10 +2553,10 @@
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="56"/>
+      <c r="C51" s="74"/>
       <c r="E51" s="87"/>
       <c r="F51" s="87"/>
       <c r="H51" s="30" t="s">
@@ -2452,10 +2567,10 @@
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="55" t="s">
+      <c r="B52" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="56"/>
+      <c r="C52" s="74"/>
       <c r="E52" s="87"/>
       <c r="F52" s="87"/>
       <c r="H52" s="30" t="s">
@@ -2466,10 +2581,10 @@
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="55" t="s">
+      <c r="B53" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="56"/>
+      <c r="C53" s="74"/>
       <c r="E53" s="87"/>
       <c r="F53" s="87"/>
       <c r="H53" s="30" t="s">
@@ -2480,10 +2595,10 @@
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="56"/>
+      <c r="C54" s="74"/>
       <c r="E54" s="87"/>
       <c r="F54" s="87"/>
       <c r="H54" s="31" t="s">
@@ -2494,19 +2609,19 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="55" t="s">
+      <c r="B55" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="56"/>
+      <c r="C55" s="74"/>
       <c r="E55" s="87"/>
       <c r="F55" s="87"/>
       <c r="I55" s="37"/>
     </row>
     <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="C56" s="58"/>
+      <c r="C56" s="76"/>
       <c r="E56" s="87"/>
       <c r="F56" s="87"/>
       <c r="I56" s="37"/>
@@ -2541,25 +2656,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N14:O14"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="H36:I36"/>
@@ -2574,6 +2670,25 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="E31:F60"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
@@ -2584,20 +2699,216 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="90" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="90" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="89" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="89" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="89" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="89" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="89" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="89" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="89" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="89" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="89" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="89" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="89" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="89" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="89" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="89" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="89" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="89" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="89" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="89" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update:  - workorder_table  - admin_menu_sidebar.blade.php  - TdrController.php  - bd_avia_v3_a.xlsx  - tdr: index, create, edit
</commit_message>
<xml_diff>
--- a/public/data/bd_avia_v3_a.xlsx
+++ b/public/data/bd_avia_v3_a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\avia\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A62A69-D128-4291-91FD-2054DD980855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B93E55B-E95F-40F6-A344-72AAC56FC8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="172">
   <si>
     <t>workorder</t>
   </si>
@@ -266,18 +266,6 @@
   </si>
   <si>
     <t>ipl_num</t>
-  </si>
-  <si>
-    <t>PARTS MISSING UPON ARRIVAL AS INDICATED ON PARTS LIST</t>
-  </si>
-  <si>
-    <t>UNIT RECEIVED COMPLETELY DISASSEMBLED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?  DISASSEMBLED UPON ARRIVAL </t>
-  </si>
-  <si>
-    <t>BUSHINGS WORN BEYOND LIMITS AS INDICATED ON PARTS LIST</t>
   </si>
   <si>
     <t>Damage</t>
@@ -551,9 +539,6 @@
     <t xml:space="preserve"> PISTON</t>
   </si>
   <si>
-    <t>inspect_std</t>
-  </si>
-  <si>
     <t>conditions</t>
   </si>
   <si>
@@ -573,13 +558,34 @@
   </si>
   <si>
     <t>process</t>
+  </si>
+  <si>
+    <t>extermal_damage</t>
+  </si>
+  <si>
+    <t>received_disassembly</t>
+  </si>
+  <si>
+    <t>nameplate_missing</t>
+  </si>
+  <si>
+    <t>part_missing</t>
+  </si>
+  <si>
+    <t>preliminary_test_false</t>
+  </si>
+  <si>
+    <t>extra_parts</t>
+  </si>
+  <si>
+    <t>disassembly_upon_arrival</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,14 +671,8 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,14 +697,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -971,30 +965,8 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1008,12 +980,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1105,9 +1125,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1147,13 +1164,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1180,7 +1191,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1195,83 +1206,86 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1559,8 +1573,8 @@
   </sheetPr>
   <dimension ref="B1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1583,7 @@
     <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="3" customWidth="1"/>
     <col min="4" max="4" width="1.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="28" style="3" customWidth="1"/>
     <col min="7" max="7" width="1.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" style="1" customWidth="1"/>
@@ -1587,27 +1601,27 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="E2" s="84" t="s">
+      <c r="C2" s="74"/>
+      <c r="E2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="H2" s="73" t="s">
+      <c r="F2" s="74"/>
+      <c r="H2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="74"/>
+      <c r="I2" s="63"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="70"/>
-      <c r="N2" s="73" t="s">
+      <c r="L2" s="59"/>
+      <c r="N2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="74"/>
+      <c r="O2" s="63"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1685,10 +1699,10 @@
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="H5" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="8" t="s">
@@ -1726,10 +1740,10 @@
       <c r="L6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="75" t="s">
+      <c r="N6" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="76"/>
+      <c r="O6" s="65"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1773,10 +1787,10 @@
       <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="76"/>
+      <c r="I8" s="65"/>
       <c r="J8" s="2"/>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -1830,10 +1844,10 @@
         <v>66</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="72"/>
+      <c r="O10" s="61"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -1926,16 +1940,16 @@
         <v>53</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="N14" s="71" t="s">
+      <c r="N14" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="72"/>
+      <c r="O14" s="61"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
@@ -1945,7 +1959,7 @@
         <v>53</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>18</v>
@@ -1965,7 +1979,7 @@
         <v>53</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>18</v>
@@ -1977,15 +1991,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="81" t="s">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="E17" s="24" t="s">
+      <c r="C17" s="71"/>
+      <c r="E17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="11" t="s">
         <v>53</v>
       </c>
       <c r="H17" s="6" t="s">
@@ -2004,18 +2018,22 @@
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
+      <c r="E18" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="H18" s="6" t="s">
         <v>71</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="71" t="s">
+      <c r="N18" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="72"/>
+      <c r="O18" s="61"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
@@ -2024,6 +2042,12 @@
       <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="E19" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="H19" s="14" t="s">
         <v>72</v>
       </c>
@@ -2044,6 +2068,12 @@
       <c r="C20" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="E20" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N20" s="6" t="s">
         <v>25</v>
       </c>
@@ -2058,8 +2088,12 @@
       <c r="C21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="E21" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N21" s="6" t="s">
         <v>57</v>
       </c>
@@ -2074,8 +2108,12 @@
       <c r="C22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N22" s="6" t="s">
         <v>58</v>
       </c>
@@ -2090,11 +2128,17 @@
       <c r="C23" s="11" t="s">
         <v>53</v>
       </c>
+      <c r="E23" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N23" s="6" t="s">
         <v>59</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2104,21 +2148,27 @@
       <c r="C24" s="25" t="s">
         <v>53</v>
       </c>
+      <c r="E24" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="N24" s="12" t="s">
         <v>9</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
       <c r="D25" s="21"/>
-      <c r="N25" s="71" t="s">
+      <c r="N25" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="72"/>
+      <c r="O25" s="61"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
@@ -2141,32 +2191,32 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="83"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="79" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="75"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="I28" s="69"/>
+      <c r="K28" s="68" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="I28" s="80"/>
-      <c r="K28" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="L28" s="80"/>
+      <c r="L28" s="69"/>
       <c r="N28" s="12"/>
       <c r="O28" s="18"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -2178,41 +2228,45 @@
       <c r="H29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="37" t="s">
+      <c r="I29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="39" t="s">
+      <c r="K29" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="37" t="s">
+      <c r="L29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="71" t="s">
+      <c r="N29" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="72"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="48" t="s">
+      <c r="O29" s="61"/>
+    </row>
+    <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="77" t="s">
         <v>18</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="37" t="s">
+      <c r="I30" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
+      <c r="K30" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="84" t="s">
+        <v>18</v>
+      </c>
       <c r="N30" s="4" t="s">
         <v>20</v>
       </c>
@@ -2221,27 +2275,27 @@
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="67"/>
+      <c r="E31" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="79"/>
       <c r="H31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="37" t="s">
+      <c r="I31" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="K31" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="L31" s="38" t="s">
-        <v>18</v>
+      <c r="K31" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="N31" s="6" t="s">
         <v>55</v>
@@ -2251,70 +2305,64 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="81"/>
       <c r="H32" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="K32" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="L32" s="38" t="s">
+      <c r="K32" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="L32" s="32" t="s">
         <v>18</v>
       </c>
       <c r="N32" s="12"/>
       <c r="O32" s="18"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="81"/>
       <c r="H33" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="K33" s="48" t="s">
+      <c r="K33" s="46" t="s">
         <v>69</v>
       </c>
       <c r="L33" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="71" t="s">
+      <c r="N33" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="72"/>
+      <c r="O33" s="61"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="52"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="23"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="81"/>
       <c r="H34" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="I34" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="K34" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="L34" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="36" t="s">
         <v>53</v>
       </c>
       <c r="N34" s="4" t="s">
@@ -2325,14 +2373,14 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="52"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="23"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="68"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="81"/>
       <c r="H35" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I35" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="36" t="s">
         <v>53</v>
       </c>
       <c r="N35" s="14" t="s">
@@ -2343,23 +2391,27 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="35"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="I36" s="36"/>
-      <c r="N36" s="77" t="s">
+      <c r="B36" s="41"/>
+      <c r="C36" s="42"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="81"/>
+      <c r="I36" s="35"/>
+      <c r="N36" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="78"/>
-    </row>
-    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="35"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="H37" s="58" t="s">
+      <c r="O36" s="67"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="56" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="81"/>
+      <c r="H37" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="I37" s="59"/>
+      <c r="I37" s="56"/>
       <c r="N37" s="4" t="s">
         <v>20</v>
       </c>
@@ -2368,16 +2420,18 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="C38" s="60"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
+      <c r="B38" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="80"/>
+      <c r="F38" s="81"/>
       <c r="H38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="37" t="s">
+      <c r="I38" s="36" t="s">
         <v>22</v>
       </c>
       <c r="N38" s="6" t="s">
@@ -2389,48 +2443,47 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
+        <v>5</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="80"/>
+      <c r="F39" s="81"/>
       <c r="H39" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I39" s="38" t="s">
+      <c r="I39" s="37" t="s">
         <v>27</v>
       </c>
       <c r="N39" s="12"/>
       <c r="O39" s="13"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="68"/>
-      <c r="F40" s="68"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="13"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="81"/>
       <c r="H40" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="38" t="s">
+      <c r="I40" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="N40" s="77" t="s">
+      <c r="N40" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="O40" s="78"/>
-    </row>
-    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="35"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
+      <c r="O40" s="67"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="E41" s="80"/>
+      <c r="F41" s="81"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="36"/>
+      <c r="I41" s="35"/>
       <c r="N41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2439,17 +2492,17 @@
       </c>
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="52"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="81"/>
+      <c r="H42" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="62"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="H42" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="I42" s="41" t="s">
-        <v>85</v>
+      <c r="I42" s="40" t="s">
+        <v>81</v>
       </c>
       <c r="N42" s="14" t="s">
         <v>5</v>
@@ -2459,241 +2512,196 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="64"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
+      <c r="B43" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="52"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="81"/>
       <c r="H43" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I43" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="52"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="81"/>
+      <c r="H44" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="52"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="81"/>
+      <c r="H45" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="I43" s="41" t="s">
+      <c r="I45" s="40" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="64"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="H44" s="29" t="s">
+    <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="54"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="81"/>
+      <c r="H46" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="41" t="s">
+      <c r="I46" s="40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="65" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="66"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="68"/>
-      <c r="H45" s="29" t="s">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E47" s="80"/>
+      <c r="F47" s="81"/>
+      <c r="H47" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="I45" s="41" t="s">
+      <c r="I47" s="40" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="42"/>
-      <c r="C46" s="43"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="68"/>
-      <c r="H46" s="29" t="s">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E48" s="80"/>
+      <c r="F48" s="81"/>
+      <c r="H48" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="I46" s="41" t="s">
+      <c r="I48" s="40" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C47" s="60"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="68"/>
-      <c r="H47" s="29" t="s">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="80"/>
+      <c r="F49" s="81"/>
+      <c r="H49" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I47" s="41" t="s">
+      <c r="I49" s="40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="H48" s="29" t="s">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="80"/>
+      <c r="F50" s="81"/>
+      <c r="H50" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="I48" s="41" t="s">
+      <c r="I50" s="40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="H49" s="29" t="s">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="80"/>
+      <c r="F51" s="81"/>
+      <c r="H51" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="I49" s="41" t="s">
+      <c r="I51" s="40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="35"/>
-      <c r="C50" s="13"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="H50" s="29" t="s">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E52" s="80"/>
+      <c r="F52" s="81"/>
+      <c r="H52" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="I50" s="41" t="s">
+      <c r="I52" s="40" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="C51" s="55"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="H51" s="29" t="s">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E53" s="80"/>
+      <c r="F53" s="81"/>
+      <c r="H53" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="I51" s="41" t="s">
+      <c r="I53" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="55"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="68"/>
-      <c r="H52" s="29" t="s">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E54" s="80"/>
+      <c r="F54" s="81"/>
+      <c r="H54" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I52" s="41" t="s">
+      <c r="I54" s="40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="80"/>
+      <c r="F55" s="81"/>
+      <c r="H55" s="30" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="55"/>
-      <c r="E53" s="68"/>
-      <c r="F53" s="68"/>
-      <c r="H53" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="I53" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="55"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68"/>
-      <c r="H54" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="I54" s="41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="55"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="H55" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="I55" s="44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" s="57"/>
-      <c r="E56" s="68"/>
-      <c r="F56" s="68"/>
-      <c r="I56" s="36"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="35"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="35"/>
-      <c r="E58" s="68"/>
-      <c r="F58" s="68"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="35"/>
-      <c r="E59" s="68"/>
-      <c r="F59" s="68"/>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="45"/>
-      <c r="C60" s="46"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="47"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E61" s="68"/>
-      <c r="F61" s="68"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E62" s="68"/>
-      <c r="F62" s="68"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E63" s="68"/>
-      <c r="F63" s="68"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E64" s="68"/>
-      <c r="F64" s="68"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E65" s="68"/>
-      <c r="F65" s="68"/>
+      <c r="I55" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E56" s="80"/>
+      <c r="F56" s="81"/>
+      <c r="I56" s="35"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E57" s="80"/>
+      <c r="F57" s="81"/>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E58" s="80"/>
+      <c r="F58" s="81"/>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E59" s="80"/>
+      <c r="F59" s="81"/>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="44"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="81"/>
+      <c r="G60" s="44"/>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E61" s="80"/>
+      <c r="F61" s="81"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E62" s="80"/>
+      <c r="F62" s="81"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E63" s="80"/>
+      <c r="F63" s="81"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E64" s="80"/>
+      <c r="F64" s="81"/>
+    </row>
+    <row r="65" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="82"/>
+      <c r="F65" s="83"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="29">
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B28:C28"/>
@@ -2714,19 +2722,14 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="E31:F65"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
@@ -2758,193 +2761,193 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>125</v>
+      <c r="A2" s="50" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
-        <v>126</v>
+      <c r="A3" s="50" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add edit & delete workorders
</commit_message>
<xml_diff>
--- a/public/data/bd_avia_v3_a.xlsx
+++ b/public/data/bd_avia_v3_a.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\avia\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\avia.loc\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD87E10-B74A-4273-BF82-0585666E0B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -518,9 +517,6 @@
   </si>
   <si>
     <t>process</t>
-  </si>
-  <si>
-    <t>extermal_damage</t>
   </si>
   <si>
     <t>received_disassembly</t>
@@ -599,11 +595,14 @@
   <si>
     <t>use_process_forms</t>
   </si>
+  <si>
+    <t>external_damage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1210,58 +1209,22 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1297,28 +1260,64 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Form # 003" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal_Form # 003" xfId="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1595,14 +1594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,27 +1628,27 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="E2" s="59" t="s">
+      <c r="C2" s="87"/>
+      <c r="E2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="H2" s="54" t="s">
+      <c r="F2" s="87"/>
+      <c r="H2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="55"/>
+      <c r="I2" s="76"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="N2" s="54" t="s">
+      <c r="L2" s="72"/>
+      <c r="N2" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="55"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1768,10 +1767,10 @@
       <c r="L6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="65" t="s">
+      <c r="N6" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="66"/>
+      <c r="O6" s="78"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1815,10 +1814,10 @@
       <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="66"/>
+      <c r="I8" s="78"/>
       <c r="J8" s="2"/>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -1872,10 +1871,10 @@
         <v>66</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="N10" s="67" t="s">
+      <c r="N10" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="68"/>
+      <c r="O10" s="74"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -1974,10 +1973,10 @@
         <v>18</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="N14" s="67" t="s">
+      <c r="N14" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="68"/>
+      <c r="O14" s="74"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
@@ -2020,10 +2019,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="84"/>
       <c r="E17" s="10" t="s">
         <v>6</v>
       </c>
@@ -2046,10 +2045,10 @@
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="86" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" s="87" t="s">
+      <c r="E18" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="58" t="s">
         <v>67</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -2058,10 +2057,10 @@
       <c r="I18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="67" t="s">
+      <c r="N18" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="68"/>
+      <c r="O18" s="74"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
@@ -2070,10 +2069,10 @@
       <c r="C19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="86" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="87" t="s">
+      <c r="E19" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="58" t="s">
         <v>67</v>
       </c>
       <c r="H19" s="14" t="s">
@@ -2096,10 +2095,10 @@
       <c r="C20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="86" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="87" t="s">
+      <c r="E20" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="58" t="s">
         <v>67</v>
       </c>
       <c r="N20" s="6" t="s">
@@ -2116,10 +2115,10 @@
       <c r="C21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="86" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="87" t="s">
+      <c r="E21" s="57" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" s="58" t="s">
         <v>67</v>
       </c>
       <c r="N21" s="6" t="s">
@@ -2136,10 +2135,10 @@
       <c r="C22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="86" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" s="87" t="s">
+      <c r="E22" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="58" t="s">
         <v>67</v>
       </c>
       <c r="N22" s="6" t="s">
@@ -2156,10 +2155,10 @@
       <c r="C23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="86" t="s">
-        <v>169</v>
-      </c>
-      <c r="F23" s="87" t="s">
+      <c r="E23" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="58" t="s">
         <v>67</v>
       </c>
       <c r="N23" s="6" t="s">
@@ -2176,10 +2175,10 @@
       <c r="C24" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="F24" s="85" t="s">
+      <c r="E24" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="56" t="s">
         <v>67</v>
       </c>
       <c r="N24" s="12" t="s">
@@ -2193,10 +2192,10 @@
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
       <c r="D25" s="21"/>
-      <c r="N25" s="67" t="s">
+      <c r="N25" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="68"/>
+      <c r="O25" s="74"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
@@ -2219,24 +2218,24 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="58"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="33"/>
-      <c r="E28" s="61" t="s">
+      <c r="E28" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="F28" s="62"/>
+      <c r="F28" s="88"/>
       <c r="G28" s="33"/>
-      <c r="H28" s="61" t="s">
+      <c r="H28" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="I28" s="69"/>
-      <c r="K28" s="61" t="s">
+      <c r="I28" s="82"/>
+      <c r="K28" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="L28" s="69"/>
+      <c r="L28" s="82"/>
       <c r="N28" s="12"/>
       <c r="O28" s="18"/>
     </row>
@@ -2265,10 +2264,10 @@
       <c r="L29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="67" t="s">
+      <c r="N29" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="68"/>
+      <c r="O29" s="74"/>
     </row>
     <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="45" t="s">
@@ -2303,16 +2302,16 @@
       </c>
     </row>
     <row r="31" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="84" t="s">
+      <c r="B31" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="79" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="80"/>
+      <c r="E31" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="68"/>
       <c r="H31" s="4" t="s">
         <v>11</v>
       </c>
@@ -2339,8 +2338,8 @@
       <c r="C32" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="81"/>
-      <c r="F32" s="82"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
       <c r="H32" s="4" t="s">
         <v>112</v>
       </c>
@@ -2363,8 +2362,8 @@
       <c r="C33" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="81"/>
-      <c r="F33" s="82"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
       <c r="H33" s="4" t="s">
         <v>113</v>
       </c>
@@ -2377,10 +2376,10 @@
       <c r="L33" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="67" t="s">
+      <c r="N33" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="68"/>
+      <c r="O33" s="74"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="46" t="s">
@@ -2389,8 +2388,8 @@
       <c r="C34" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="81"/>
-      <c r="F34" s="82"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
       <c r="H34" s="4" t="s">
         <v>160</v>
       </c>
@@ -2407,8 +2406,8 @@
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="49"/>
       <c r="C35" s="23"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="82"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
       <c r="H35" s="4" t="s">
         <v>161</v>
       </c>
@@ -2425,28 +2424,28 @@
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="49"/>
       <c r="C36" s="23"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="82"/>
-      <c r="H36" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="I36" s="83" t="s">
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
+      <c r="H36" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="I36" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="N36" s="63" t="s">
+      <c r="N36" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="64"/>
+      <c r="O36" s="80"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="82"/>
-      <c r="H37" s="83" t="s">
-        <v>173</v>
-      </c>
-      <c r="I37" s="84" t="s">
+      <c r="E37" s="69"/>
+      <c r="F37" s="70"/>
+      <c r="H37" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="55" t="s">
         <v>67</v>
       </c>
       <c r="N37" s="4" t="s">
@@ -2457,16 +2456,16 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="77" t="s">
+      <c r="B38" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="78"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="82"/>
-      <c r="H38" s="83" t="s">
-        <v>177</v>
-      </c>
-      <c r="I38" s="84" t="s">
+      <c r="C38" s="66"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="H38" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="I38" s="55" t="s">
         <v>67</v>
       </c>
       <c r="N38" s="6" t="s">
@@ -2483,12 +2482,12 @@
       <c r="C39" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="81"/>
-      <c r="F39" s="82"/>
-      <c r="H39" s="83" t="s">
-        <v>174</v>
-      </c>
-      <c r="I39" s="84" t="s">
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="H39" s="54" t="s">
+        <v>173</v>
+      </c>
+      <c r="I39" s="55" t="s">
         <v>67</v>
       </c>
       <c r="N39" s="12"/>
@@ -2501,24 +2500,24 @@
       <c r="C40" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="81"/>
-      <c r="F40" s="82"/>
-      <c r="H40" s="83" t="s">
-        <v>176</v>
-      </c>
-      <c r="I40" s="84" t="s">
+      <c r="E40" s="69"/>
+      <c r="F40" s="70"/>
+      <c r="H40" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="N40" s="63" t="s">
+      <c r="N40" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="O40" s="64"/>
+      <c r="O40" s="80"/>
     </row>
     <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="34"/>
       <c r="C41" s="13"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="82"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="70"/>
       <c r="I41" s="35"/>
       <c r="N41" s="4" t="s">
         <v>20</v>
@@ -2528,16 +2527,16 @@
       </c>
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="72" t="s">
+      <c r="B42" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="73"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="82"/>
-      <c r="H42" s="76" t="s">
+      <c r="C42" s="61"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="70"/>
+      <c r="H42" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="I42" s="77"/>
+      <c r="I42" s="65"/>
       <c r="N42" s="14" t="s">
         <v>5</v>
       </c>
@@ -2546,12 +2545,12 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="72" t="s">
+      <c r="B43" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="73"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
+      <c r="C43" s="61"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
       <c r="H43" s="4" t="s">
         <v>20</v>
       </c>
@@ -2560,12 +2559,12 @@
       </c>
     </row>
     <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="73"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="82"/>
+      <c r="C44" s="61"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
       <c r="H44" s="27" t="s">
         <v>5</v>
       </c>
@@ -2574,12 +2573,12 @@
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="73"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="82"/>
+      <c r="C45" s="61"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="70"/>
       <c r="H45" s="27" t="s">
         <v>25</v>
       </c>
@@ -2588,22 +2587,22 @@
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="73"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="82"/>
+      <c r="C46" s="61"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="70"/>
       <c r="H46" s="12"/>
       <c r="I46" s="35"/>
     </row>
     <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="82"/>
+      <c r="C47" s="63"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="70"/>
       <c r="H47" s="29" t="s">
         <v>80</v>
       </c>
@@ -2612,8 +2611,8 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E48" s="81"/>
-      <c r="F48" s="82"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="70"/>
       <c r="H48" s="29" t="s">
         <v>82</v>
       </c>
@@ -2622,8 +2621,8 @@
       </c>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="81"/>
-      <c r="F49" s="82"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="70"/>
       <c r="H49" s="29" t="s">
         <v>84</v>
       </c>
@@ -2632,8 +2631,8 @@
       </c>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="81"/>
-      <c r="F50" s="82"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="70"/>
       <c r="H50" s="29" t="s">
         <v>86</v>
       </c>
@@ -2642,8 +2641,8 @@
       </c>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="70"/>
       <c r="H51" s="29" t="s">
         <v>88</v>
       </c>
@@ -2652,8 +2651,8 @@
       </c>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E52" s="81"/>
-      <c r="F52" s="82"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="70"/>
       <c r="H52" s="29" t="s">
         <v>90</v>
       </c>
@@ -2662,8 +2661,8 @@
       </c>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E53" s="81"/>
-      <c r="F53" s="82"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="70"/>
       <c r="H53" s="29" t="s">
         <v>92</v>
       </c>
@@ -2672,8 +2671,8 @@
       </c>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E54" s="81"/>
-      <c r="F54" s="82"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="70"/>
       <c r="H54" s="29" t="s">
         <v>94</v>
       </c>
@@ -2682,8 +2681,8 @@
       </c>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E55" s="81"/>
-      <c r="F55" s="82"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="70"/>
       <c r="H55" s="29" t="s">
         <v>96</v>
       </c>
@@ -2692,8 +2691,8 @@
       </c>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E56" s="81"/>
-      <c r="F56" s="82"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="70"/>
       <c r="H56" s="29" t="s">
         <v>98</v>
       </c>
@@ -2702,8 +2701,8 @@
       </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E57" s="81"/>
-      <c r="F57" s="82"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="70"/>
       <c r="H57" s="29" t="s">
         <v>100</v>
       </c>
@@ -2712,8 +2711,8 @@
       </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E58" s="81"/>
-      <c r="F58" s="82"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="70"/>
       <c r="H58" s="29" t="s">
         <v>102</v>
       </c>
@@ -2722,8 +2721,8 @@
       </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E59" s="81"/>
-      <c r="F59" s="82"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="70"/>
       <c r="H59" s="29" t="s">
         <v>104</v>
       </c>
@@ -2732,8 +2731,8 @@
       </c>
     </row>
     <row r="60" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="81"/>
-      <c r="F60" s="82"/>
+      <c r="E60" s="69"/>
+      <c r="F60" s="70"/>
       <c r="G60" s="44"/>
       <c r="H60" s="30" t="s">
         <v>105</v>
@@ -2743,31 +2742,30 @@
       </c>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E61" s="81"/>
-      <c r="F61" s="82"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="70"/>
       <c r="I61" s="35"/>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E62" s="81"/>
-      <c r="F62" s="82"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="70"/>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E63" s="81"/>
-      <c r="F63" s="82"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="70"/>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E64" s="81"/>
-      <c r="F64" s="82"/>
+      <c r="E64" s="69"/>
+      <c r="F64" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E31:F64"/>
     <mergeCell ref="K2:L2"/>
@@ -2784,12 +2782,13 @@
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="K28:L28"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
@@ -2798,7 +2797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>

<commit_message>
TDR: inspection - continue
</commit_message>
<xml_diff>
--- a/public/data/bd_avia_v3_a.xlsx
+++ b/public/data/bd_avia_v3_a.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\avia.loc\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\avia\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E00AD9-B42C-43F8-B129-0C2DFB87A2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="25770" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="181">
   <si>
     <t>workorder</t>
   </si>
@@ -598,12 +599,21 @@
   <si>
     <t>external_damage</t>
   </si>
+  <si>
+    <t>new_parts</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>integer, UNSIGNED , default 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +707,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -724,7 +749,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1043,12 +1068,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1227,6 +1265,78 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1242,82 +1352,22 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal_Form # 003" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Form # 003" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1594,14 +1644,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O64"/>
+  <dimension ref="B1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,27 +1678,27 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="E2" s="86" t="s">
+      <c r="C2" s="66"/>
+      <c r="E2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="87"/>
-      <c r="H2" s="75" t="s">
+      <c r="F2" s="66"/>
+      <c r="H2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="76"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="71" t="s">
+      <c r="K2" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="72"/>
-      <c r="N2" s="75" t="s">
+      <c r="L2" s="76"/>
+      <c r="N2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="76"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1767,10 +1817,10 @@
       <c r="L6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="77" t="s">
+      <c r="N6" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="78"/>
+      <c r="O6" s="80"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1814,10 +1864,10 @@
       <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="78"/>
+      <c r="I8" s="80"/>
       <c r="J8" s="2"/>
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
@@ -1871,10 +1921,10 @@
         <v>66</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="N10" s="73" t="s">
+      <c r="N10" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="74"/>
+      <c r="O10" s="78"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -1973,10 +2023,10 @@
         <v>18</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="N14" s="73" t="s">
+      <c r="N14" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="74"/>
+      <c r="O14" s="78"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
@@ -2019,10 +2069,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="84"/>
+      <c r="C17" s="63"/>
       <c r="E17" s="10" t="s">
         <v>6</v>
       </c>
@@ -2057,10 +2107,10 @@
       <c r="I18" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="73" t="s">
+      <c r="N18" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="74"/>
+      <c r="O18" s="78"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
@@ -2135,10 +2185,10 @@
       <c r="C22" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="58" t="s">
+      <c r="E22" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="90" t="s">
         <v>67</v>
       </c>
       <c r="N22" s="6" t="s">
@@ -2156,7 +2206,7 @@
         <v>53</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F23" s="58" t="s">
         <v>67</v>
@@ -2175,10 +2225,10 @@
       <c r="C24" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="56" t="s">
+      <c r="E24" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" s="58" t="s">
         <v>67</v>
       </c>
       <c r="N24" s="12" t="s">
@@ -2188,14 +2238,20 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
       <c r="D25" s="21"/>
-      <c r="N25" s="73" t="s">
+      <c r="E25" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N25" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="74"/>
+      <c r="O25" s="78"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
@@ -2208,8 +2264,6 @@
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
       <c r="N27" s="6" t="s">
         <v>5</v>
       </c>
@@ -2218,24 +2272,22 @@
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="85" t="s">
+      <c r="B28" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="85"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="33"/>
-      <c r="E28" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="88"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="33"/>
-      <c r="H28" s="81" t="s">
+      <c r="H28" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="I28" s="82"/>
-      <c r="K28" s="81" t="s">
+      <c r="I28" s="83"/>
+      <c r="K28" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="L28" s="82"/>
+      <c r="L28" s="83"/>
       <c r="N28" s="12"/>
       <c r="O28" s="18"/>
     </row>
@@ -2246,12 +2298,10 @@
       <c r="C29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="E29" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" s="68"/>
       <c r="H29" s="4" t="s">
         <v>20</v>
       </c>
@@ -2264,23 +2314,23 @@
       <c r="L29" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="73" t="s">
+      <c r="N29" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="O29" s="74"/>
-    </row>
-    <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O29" s="78"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="45" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="52" t="s">
-        <v>18</v>
+      <c r="E30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>41</v>
@@ -2301,17 +2351,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="54" t="s">
         <v>170</v>
       </c>
       <c r="C31" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="F31" s="68"/>
+      <c r="E31" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="52" t="s">
+        <v>18</v>
+      </c>
       <c r="H31" s="4" t="s">
         <v>11</v>
       </c>
@@ -2338,8 +2390,10 @@
       <c r="C32" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="69"/>
-      <c r="F32" s="70"/>
+      <c r="E32" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="72"/>
       <c r="H32" s="4" t="s">
         <v>112</v>
       </c>
@@ -2362,8 +2416,8 @@
       <c r="C33" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="69"/>
-      <c r="F33" s="70"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="74"/>
       <c r="H33" s="4" t="s">
         <v>113</v>
       </c>
@@ -2376,10 +2430,10 @@
       <c r="L33" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N33" s="73" t="s">
+      <c r="N33" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="74"/>
+      <c r="O33" s="78"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="46" t="s">
@@ -2388,8 +2442,8 @@
       <c r="C34" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="69"/>
-      <c r="F34" s="70"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="74"/>
       <c r="H34" s="4" t="s">
         <v>160</v>
       </c>
@@ -2406,8 +2460,8 @@
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="49"/>
       <c r="C35" s="23"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="70"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="74"/>
       <c r="H35" s="4" t="s">
         <v>161</v>
       </c>
@@ -2424,29 +2478,29 @@
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="49"/>
       <c r="C36" s="23"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="70"/>
-      <c r="H36" s="54" t="s">
-        <v>171</v>
-      </c>
-      <c r="I36" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="N36" s="79" t="s">
+      <c r="E36" s="73"/>
+      <c r="F36" s="74"/>
+      <c r="H36" s="91" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="N36" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="80"/>
+      <c r="O36" s="82"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="70"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="74"/>
       <c r="H37" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="I37" s="55" t="s">
-        <v>67</v>
+        <v>171</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>18</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>20</v>
@@ -2456,14 +2510,14 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="65" t="s">
+      <c r="B38" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="66"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="74"/>
       <c r="H38" s="54" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I38" s="55" t="s">
         <v>67</v>
@@ -2482,10 +2536,10 @@
       <c r="C39" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="69"/>
-      <c r="F39" s="70"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="74"/>
       <c r="H39" s="54" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I39" s="55" t="s">
         <v>67</v>
@@ -2500,25 +2554,30 @@
       <c r="C40" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="69"/>
-      <c r="F40" s="70"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="74"/>
       <c r="H40" s="54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I40" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="N40" s="79" t="s">
+      <c r="N40" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="O40" s="80"/>
-    </row>
-    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O40" s="82"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="34"/>
       <c r="C41" s="13"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="70"/>
-      <c r="I41" s="35"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="74"/>
+      <c r="H41" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I41" s="55" t="s">
+        <v>67</v>
+      </c>
       <c r="N41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2527,16 +2586,13 @@
       </c>
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="70"/>
-      <c r="H42" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I42" s="65"/>
+      <c r="C42" s="85"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="74"/>
+      <c r="I42" s="35"/>
       <c r="N42" s="14" t="s">
         <v>5</v>
       </c>
@@ -2545,229 +2601,238 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="60" t="s">
+      <c r="B43" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="61"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="70"/>
-      <c r="H43" s="4" t="s">
+      <c r="C43" s="85"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="74"/>
+      <c r="H43" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="69"/>
+    </row>
+    <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="85"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="74"/>
+      <c r="H44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I44" s="36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="70"/>
-      <c r="H44" s="27" t="s">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="85"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="74"/>
+      <c r="H45" s="27" t="s">
         <v>5</v>
-      </c>
-      <c r="I44" s="37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="70"/>
-      <c r="H45" s="27" t="s">
-        <v>25</v>
       </c>
       <c r="I45" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="70"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="35"/>
+      <c r="C46" s="85"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="74"/>
+      <c r="H46" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="37" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
-      <c r="H47" s="29" t="s">
+      <c r="C47" s="87"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="74"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="35"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E48" s="73"/>
+      <c r="F48" s="74"/>
+      <c r="H48" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="I48" s="40" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E48" s="69"/>
-      <c r="F48" s="70"/>
-      <c r="H48" s="29" t="s">
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="73"/>
+      <c r="F49" s="74"/>
+      <c r="H49" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="40" t="s">
+      <c r="I49" s="40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="69"/>
-      <c r="F49" s="70"/>
-      <c r="H49" s="29" t="s">
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="73"/>
+      <c r="F50" s="74"/>
+      <c r="H50" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="I49" s="40" t="s">
+      <c r="I50" s="40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E50" s="69"/>
-      <c r="F50" s="70"/>
-      <c r="H50" s="29" t="s">
+    <row r="51" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="73"/>
+      <c r="F51" s="74"/>
+      <c r="H51" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="I50" s="40" t="s">
+      <c r="I51" s="40" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E51" s="69"/>
-      <c r="F51" s="70"/>
-      <c r="H51" s="29" t="s">
+    <row r="52" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E52" s="73"/>
+      <c r="F52" s="74"/>
+      <c r="H52" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="I51" s="40" t="s">
+      <c r="I52" s="40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E52" s="69"/>
-      <c r="F52" s="70"/>
-      <c r="H52" s="29" t="s">
+    <row r="53" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E53" s="73"/>
+      <c r="F53" s="74"/>
+      <c r="H53" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="I52" s="40" t="s">
+      <c r="I53" s="40" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E53" s="69"/>
-      <c r="F53" s="70"/>
-      <c r="H53" s="29" t="s">
+    <row r="54" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E54" s="73"/>
+      <c r="F54" s="74"/>
+      <c r="H54" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="I53" s="40" t="s">
+      <c r="I54" s="40" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E54" s="69"/>
-      <c r="F54" s="70"/>
-      <c r="H54" s="29" t="s">
+    <row r="55" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E55" s="73"/>
+      <c r="F55" s="74"/>
+      <c r="H55" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I54" s="40" t="s">
+      <c r="I55" s="40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E55" s="69"/>
-      <c r="F55" s="70"/>
-      <c r="H55" s="29" t="s">
+    <row r="56" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E56" s="73"/>
+      <c r="F56" s="74"/>
+      <c r="H56" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="I55" s="40" t="s">
+      <c r="I56" s="40" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E56" s="69"/>
-      <c r="F56" s="70"/>
-      <c r="H56" s="29" t="s">
+    <row r="57" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E57" s="73"/>
+      <c r="F57" s="74"/>
+      <c r="H57" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="I56" s="40" t="s">
+      <c r="I57" s="40" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E57" s="69"/>
-      <c r="F57" s="70"/>
-      <c r="H57" s="29" t="s">
+    <row r="58" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E58" s="73"/>
+      <c r="F58" s="74"/>
+      <c r="H58" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="I57" s="40" t="s">
+      <c r="I58" s="40" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E58" s="69"/>
-      <c r="F58" s="70"/>
-      <c r="H58" s="29" t="s">
+    <row r="59" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E59" s="73"/>
+      <c r="F59" s="74"/>
+      <c r="H59" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="I58" s="40" t="s">
+      <c r="I59" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E59" s="69"/>
-      <c r="F59" s="70"/>
-      <c r="H59" s="29" t="s">
+    <row r="60" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E60" s="73"/>
+      <c r="F60" s="74"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I59" s="40" t="s">
+      <c r="I60" s="40" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="69"/>
-      <c r="F60" s="70"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="30" t="s">
+    <row r="61" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="73"/>
+      <c r="F61" s="74"/>
+      <c r="H61" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="I60" s="43" t="s">
+      <c r="I61" s="43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E61" s="69"/>
-      <c r="F61" s="70"/>
-      <c r="I61" s="35"/>
-    </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E62" s="69"/>
-      <c r="F62" s="70"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="74"/>
+      <c r="I62" s="35"/>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E63" s="69"/>
-      <c r="F63" s="70"/>
+      <c r="E63" s="73"/>
+      <c r="F63" s="74"/>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E64" s="69"/>
-      <c r="F64" s="70"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="74"/>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="73"/>
+      <c r="F65" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="E31:F64"/>
+    <mergeCell ref="E32:F65"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="N18:O18"/>
@@ -2782,14 +2847,14 @@
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="K28:L28"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.05" footer="0.05"/>
   <pageSetup scale="58" orientation="landscape" verticalDpi="1200" r:id="rId1"/>
@@ -2797,7 +2862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>